<commit_message>
Added meter offsets and welltop to ground measurements
based on field visit to Sagehen on 10/18/2020
</commit_message>
<xml_diff>
--- a/data/field_observations/groundwater/Wells_Missing_Data.xlsx
+++ b/data/field_observations/groundwater/Wells_Missing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnat/Documents/GitHub/sagehen_meadows/data/field_observations/groundwater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A49024-9351-0940-B819-55B66D3FDCF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3C9D86-8F4C-4C4A-8E1A-7BCCC223910A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="1940" windowWidth="15060" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18600" yWindow="3120" windowWidth="15060" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>No top2gnd</t>
   </si>
   <si>
-    <t>KHF-XD4S</t>
-  </si>
-  <si>
     <t>KER-XE3S</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
   </si>
   <si>
     <t>KHR-XE2N</t>
-  </si>
-  <si>
-    <t>KWR-XE1N</t>
   </si>
   <si>
     <t>KEF-1</t>
@@ -525,7 +519,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C27"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -540,237 +534,216 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F24" s="3"/>
     </row>
@@ -780,13 +753,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C26" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C27" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F27" s="3"/>
     </row>

</xml_diff>